<commit_message>
Employee Number Fix and Timesheet Fix
</commit_message>
<xml_diff>
--- a/public/xls_template/timesheet.xlsx
+++ b/public/xls_template/timesheet.xlsx
@@ -19,36 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>First Name</t>
+    <t>Date Time In(YYYY-MM-DD HH:MM:SS)</t>
   </si>
   <si>
-    <t>Last Name</t>
+    <t>Date Time Out(YYY-MM-DD HH:MM:SS)</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Time In</t>
-  </si>
-  <si>
-    <t>Time Out</t>
-  </si>
-  <si>
-    <t>Date Time In(YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t>Date Time Out(YYY-MM-DD)</t>
+    <t>Emplyee Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -91,19 +76,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -434,84 +422,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="19.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22" style="2" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>